<commit_message>
Fix bug in belaege.tidy.csv
</commit_message>
<xml_diff>
--- a/00_data_raw/Rohdaten_Matrix_Belaege.xlsx
+++ b/00_data_raw/Rohdaten_Matrix_Belaege.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://zhaw-my.sharepoint.com/personal/pfeifsar_students_zhaw_ch/Documents/6. Semester MSc UnR/Thesis/R_Project/00_data_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1124" documentId="8_{E9D6D6FE-F378-4AF9-A02F-B79ECDA22C50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{223CCCB4-E8E4-473A-B1F0-8483B5E50757}"/>
+  <xr:revisionPtr revIDLastSave="1145" documentId="8_{E9D6D6FE-F378-4AF9-A02F-B79ECDA22C50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90A4D6FF-06DE-4BCC-9ECA-B74B986E2C23}"/>
   <bookViews>
-    <workbookView xWindow="-21765" yWindow="225" windowWidth="19125" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19110" yWindow="0" windowWidth="9970" windowHeight="10170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rohdaten_Belaege" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="110">
   <si>
     <t>Modulare Erneuerbarkeit</t>
   </si>
@@ -57,12 +57,6 @@
     <t>Rasengittersteine</t>
   </si>
   <si>
-    <t>25–30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15–20 </t>
-  </si>
-  <si>
     <t>40–50</t>
   </si>
   <si>
@@ -268,9 +262,6 @@
   </si>
   <si>
     <t>Die  Oberflächentemperaturen wurden aus Simulationen und Feldmessungen der Stadt Zürich (2022) - Grobökobilanz von Freiraumelementen und Xu (2018) abgeleitet, ergänzt durch Werte aus Yan (2025) zur thermischen Reflexion heller Asphaltmischungen. Als Referenzwert galt der Oberflechentemperaturwert von Asphalt von 58.4°C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Die Lebensdauer der Beläge wurde in Anlehnung an die Grobökobilanz von Freiraumelementen (Stadt Zürich, 2022) sowie die KBOB-Ökobilanzdaten 2009/1:2022 (v7.0) definiert. Ergänzende Werte zu innovativen Asphalt- und Pflasterbelägen wurden aus Xu (2018) und Yan (2025) übernommen, die die erhöhte Lebensdauer temperatur- und bindemitteloptimierter Mischungen belegen. Für ungebundene und sickerfähige Beläge wurden kürzere Nutzungszeiten nach empirischen Beobachtungen des Schwammstadt Labors Zürich et al. (2025) angesetzt. </t>
   </si>
   <si>
     <r>
@@ -389,12 +380,34 @@
   <si>
     <t>Graue Energie MW [kWh/m²]</t>
   </si>
+  <si>
+    <t>10-15</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Die Lebensdauer der Beläge wurde in Anlehnung an die Grobökobilanz von Freiraumelementen (Stadt Zürich, 2022) sowie die KBOB-Ökobilanzdaten 2009/1:2022 (v7.0) definiert. Ergänzende Werte zu innovativen Asphalt- und Pflasterbelägen wurden aus Xu (2018) und Yan (2025) übernommen, die die erhöhte Lebensdauer temperatur- und bindemitteloptimierter Mischungen belegen. Für ungebundene und sickerfähige Beläge wurden kürzere Nutzungszeiten nach empirischen Beobachtungen des Schwammstadt Labors Zürich et al. (2025) angesetzt. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Offenporiger (Sickerasphalt gemäss Kappel 2016)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Recycling Asphalt: Grobökobilanz, Sickerasphalt: Kappel (2026), Heller Asphalt: Grobökobilanz, Selbstheilenderasphalt: Abgeletet von Garcia et al (2009) (verdoppelt Lebensdauer). Betonpflaster: ökobilanz Natrusteinpflaser: Grobökobilanz, </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -458,6 +471,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -481,7 +502,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -499,6 +520,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -723,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69245AB7-8A4B-4C00-997D-6D46C1094D77}">
   <dimension ref="A1:BF27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="W4" sqref="W4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -758,94 +782,94 @@
   <sheetData>
     <row r="1" spans="1:58" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="X1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="H1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="I1" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="U1" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="V1" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="W1" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="X1" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y1" s="4" t="s">
-        <v>95</v>
-      </c>
       <c r="Z1" s="4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="AA1" s="4"/>
     </row>
     <row r="2" spans="1:58" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D2">
         <v>22.5</v>
@@ -870,7 +894,7 @@
         <v>5</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="L2">
         <v>100</v>
@@ -880,7 +904,7 @@
         <v>500</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="O2">
         <v>4</v>
@@ -900,7 +924,7 @@
         <v>225</v>
       </c>
       <c r="T2" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="U2">
         <v>295</v>
@@ -913,7 +937,7 @@
         <v>2</v>
       </c>
       <c r="X2" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="Y2">
         <v>0.6</v>
@@ -956,29 +980,29 @@
     </row>
     <row r="3" spans="1:58" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>7</v>
+      <c r="C3" s="10" t="s">
+        <v>107</v>
       </c>
       <c r="D3">
-        <v>27.5</v>
+        <v>12.5</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E11" si="0">ROUNDUP(100/D3,0)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G3">
         <v>0.35</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I3">
         <v>55.5</v>
@@ -987,17 +1011,17 @@
         <v>3</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L3">
         <v>100</v>
       </c>
       <c r="M3">
         <f t="shared" ref="M3:M11" si="1">E3*L3</f>
-        <v>400</v>
+        <v>800</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="O3">
         <v>6.5</v>
@@ -1014,23 +1038,23 @@
       </c>
       <c r="S3">
         <f t="shared" ref="S3:S11" si="3">E3*R3</f>
-        <v>240</v>
+        <v>480</v>
       </c>
       <c r="T3" s="6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="U3">
         <v>345</v>
       </c>
       <c r="V3">
         <f t="shared" ref="V3:V11" si="4">E3*U3</f>
-        <v>1380</v>
+        <v>2760</v>
       </c>
       <c r="W3" s="5">
         <v>1</v>
       </c>
       <c r="X3" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="Y3">
         <v>0.6</v>
@@ -1073,13 +1097,13 @@
     </row>
     <row r="4" spans="1:58" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D4">
         <v>17.5</v>
@@ -1095,7 +1119,7 @@
         <v>1</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I4">
         <v>54</v>
@@ -1104,7 +1128,7 @@
         <v>5</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L4">
         <v>110</v>
@@ -1114,7 +1138,7 @@
         <v>660</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="O4">
         <v>4</v>
@@ -1147,7 +1171,7 @@
         <v>1</v>
       </c>
       <c r="X4" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="Y4">
         <v>0.4</v>
@@ -1190,13 +1214,13 @@
     </row>
     <row r="5" spans="1:58" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D5">
         <v>42.5</v>
@@ -1212,7 +1236,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I5">
         <v>58.4</v>
@@ -1221,7 +1245,7 @@
         <v>5</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="L5">
         <v>138.5</v>
@@ -1241,7 +1265,7 @@
         <v>200</v>
       </c>
       <c r="Q5" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="R5">
         <v>72.5</v>
@@ -1251,7 +1275,7 @@
         <v>217.5</v>
       </c>
       <c r="T5" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="U5">
         <v>375</v>
@@ -1264,7 +1288,7 @@
         <v>0</v>
       </c>
       <c r="X5" s="6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="Y5">
         <v>0.4</v>
@@ -1307,20 +1331,20 @@
     </row>
     <row r="6" spans="1:58" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="D6">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F6" s="5">
         <v>0.6</v>
@@ -1329,7 +1353,7 @@
         <v>0.6</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I6">
         <v>47.5</v>
@@ -1338,17 +1362,17 @@
         <v>3</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L6">
         <v>350</v>
       </c>
       <c r="M6">
         <f t="shared" si="1"/>
-        <v>700</v>
+        <v>1050</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="O6">
         <v>5</v>
@@ -1358,30 +1382,30 @@
         <v>500</v>
       </c>
       <c r="Q6" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="R6">
         <v>60</v>
       </c>
       <c r="S6">
         <f t="shared" si="3"/>
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="T6" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="U6">
         <v>270</v>
       </c>
       <c r="V6">
         <f t="shared" si="4"/>
-        <v>540</v>
+        <v>810</v>
       </c>
       <c r="W6" s="5">
         <v>2</v>
       </c>
       <c r="X6" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="Y6">
         <v>0.8</v>
@@ -1424,13 +1448,13 @@
     </row>
     <row r="7" spans="1:58" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D7">
         <v>35</v>
@@ -1446,7 +1470,7 @@
         <v>1</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I7">
         <v>57.5</v>
@@ -1455,7 +1479,7 @@
         <v>4</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="L7">
         <v>100</v>
@@ -1465,7 +1489,7 @@
         <v>300</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="O7">
         <v>4</v>
@@ -1475,7 +1499,7 @@
         <v>400</v>
       </c>
       <c r="Q7" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="R7">
         <v>55</v>
@@ -1485,7 +1509,7 @@
         <v>165</v>
       </c>
       <c r="T7" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="U7">
         <v>135</v>
@@ -1498,7 +1522,7 @@
         <v>1</v>
       </c>
       <c r="X7" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="Y7">
         <v>0.6</v>
@@ -1541,13 +1565,13 @@
     </row>
     <row r="8" spans="1:58" ht="15.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D8">
         <v>30</v>
@@ -1563,7 +1587,7 @@
         <v>0.35</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I8">
         <v>50</v>
@@ -1572,7 +1596,7 @@
         <v>3</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="L8">
         <v>125</v>
@@ -1582,7 +1606,7 @@
         <v>500</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O8">
         <v>7</v>
@@ -1592,7 +1616,7 @@
         <v>700</v>
       </c>
       <c r="Q8" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="R8">
         <v>50</v>
@@ -1602,7 +1626,7 @@
         <v>200</v>
       </c>
       <c r="T8" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="U8">
         <v>175</v>
@@ -1615,7 +1639,7 @@
         <v>1</v>
       </c>
       <c r="X8" s="6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="Y8">
         <v>0.6</v>
@@ -1658,13 +1682,13 @@
     </row>
     <row r="9" spans="1:58" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D9">
         <v>17.5</v>
@@ -1680,7 +1704,7 @@
         <v>0.5</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I9">
         <v>46.5</v>
@@ -1689,7 +1713,7 @@
         <v>1</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="L9">
         <v>50</v>
@@ -1699,7 +1723,7 @@
         <v>300</v>
       </c>
       <c r="N9" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="O9">
         <v>3</v>
@@ -1709,7 +1733,7 @@
         <v>300</v>
       </c>
       <c r="Q9" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="R9">
         <v>17.5</v>
@@ -1719,7 +1743,7 @@
         <v>105</v>
       </c>
       <c r="T9" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="U9">
         <v>70</v>
@@ -1732,7 +1756,7 @@
         <v>2</v>
       </c>
       <c r="X9" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="Y9">
         <v>0.8</v>
@@ -1775,13 +1799,13 @@
     </row>
     <row r="10" spans="1:58" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D10">
         <v>15</v>
@@ -1797,7 +1821,7 @@
         <v>0.2</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I10">
         <v>49</v>
@@ -1806,7 +1830,7 @@
         <v>3</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="L10">
         <v>95</v>
@@ -1816,7 +1840,7 @@
         <v>665</v>
       </c>
       <c r="N10" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="O10">
         <v>9</v>
@@ -1826,7 +1850,7 @@
         <v>900</v>
       </c>
       <c r="Q10" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="R10">
         <v>25</v>
@@ -1836,7 +1860,7 @@
         <v>175</v>
       </c>
       <c r="T10" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="U10">
         <v>100</v>
@@ -1849,7 +1873,7 @@
         <v>1</v>
       </c>
       <c r="X10" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="Y10">
         <v>0.8</v>
@@ -1892,13 +1916,13 @@
     </row>
     <row r="11" spans="1:58" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D11">
         <v>25</v>
@@ -1908,13 +1932,13 @@
         <v>4</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G11">
         <v>0.4</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I11">
         <v>26</v>
@@ -1923,7 +1947,7 @@
         <v>3</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="L11">
         <v>100</v>
@@ -1933,7 +1957,7 @@
         <v>400</v>
       </c>
       <c r="N11" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="O11">
         <v>6</v>
@@ -1943,7 +1967,7 @@
         <v>600</v>
       </c>
       <c r="Q11" s="7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="R11">
         <v>45</v>
@@ -1953,7 +1977,7 @@
         <v>180</v>
       </c>
       <c r="T11" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="U11">
         <v>137.5</v>
@@ -1966,7 +1990,7 @@
         <v>1</v>
       </c>
       <c r="X11" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="Y11">
         <v>0.8</v>
@@ -2171,15 +2195,18 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="C3" twoDigitTextYear="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{937A7BCA-B353-42F8-9383-0330F47B4AD1}">
-  <dimension ref="A3:B14"/>
+  <dimension ref="A3:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2188,100 +2215,103 @@
     <col min="2" max="2" width="45.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" ht="51" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="51" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B3" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="161.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="104.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="133" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="75.5" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="87" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="202" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="144" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B13" s="9" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="161.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="104.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="133" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="75.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="87" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="202" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="144" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="205.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="205.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix initialkosten and initialkosten_100a in block 5 and 7
</commit_message>
<xml_diff>
--- a/00_data_raw/Rohdaten_Matrix_Belaege.xlsx
+++ b/00_data_raw/Rohdaten_Matrix_Belaege.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://zhaw-my.sharepoint.com/personal/pfeifsar_students_zhaw_ch/Documents/6. Semester MSc UnR/Thesis/R_Project/00_data_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1328" documentId="8_{E9D6D6FE-F378-4AF9-A02F-B79ECDA22C50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90B892E3-78A6-478D-AE26-B71493610707}"/>
+  <xr:revisionPtr revIDLastSave="1339" documentId="8_{E9D6D6FE-F378-4AF9-A02F-B79ECDA22C50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B64FD6C6-45CC-43BA-B4BA-2B06C5C252B3}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -230,9 +230,6 @@
     <t>Anzahl Erneuerungen [100a]</t>
   </si>
   <si>
-    <t>Unterhaltskosen [CHF/CHF/m²100a]</t>
-  </si>
-  <si>
     <t>Kosten [CHF/m²100a]</t>
   </si>
   <si>
@@ -335,6 +332,9 @@
   </si>
   <si>
     <t>nicht-erneuerbare Primärenergiebedarf bei Herstellung, Kennwerte aus Kennwerte aus KBOB-Datensatz v7.0 (2024) - Oekobilanzdaten_Baubereich, verifiziert mit Stadt Zürich 2022 - Grobökobilanz von Freiraumelementen, Eigene Annahme Ökopflastersteine gleiche Werte wie Betonpflastersteine.  Eigenen Anahme Selbstheilender Asphalt: Selbstheilender Asphalt ist ein High-Performance-Material. Die Herstellung der speziellen Additive (egal ob Kalzium-Alginat-Kapseln, Polymere, oder Stahlfasern) erfordert zusätzliche Prozessschritte und Energie im Vergleich zur reinen Bitumen- und Gesteinsproduktion (Wang et al. 2025) Wert abgeleitet von Grobökobilanz für Spezialasphalt wie z.B Grussasphalt. Sickerasphalt: Die Herstellung von Porenasphalt benötigt oft ein modifiziertes oder höheres Bindemittelvolumen (Bitumen), um die Gesteinskörner an den Kontaktpunkten stabil zu verkleben. Daher liegen die Werte leicht über dem Standard-Asphalt Schwammstadt Labor Zürich.</t>
+  </si>
+  <si>
+    <t>Unterhaltskosten [CHF/CHF/m²100a]</t>
   </si>
 </sst>
 </file>
@@ -673,14 +673,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69245AB7-8A4B-4C00-997D-6D46C1094D77}">
   <dimension ref="A1:BF27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1"/>
+    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="V10" sqref="V10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="54.26953125" customWidth="1"/>
-    <col min="2" max="2" width="42" customWidth="1"/>
+    <col min="1" max="1" width="15.7265625" customWidth="1"/>
+    <col min="2" max="2" width="40.6328125" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="19.36328125" customWidth="1"/>
     <col min="5" max="5" width="25.7265625" customWidth="1"/>
@@ -695,14 +695,15 @@
     <col min="14" max="14" width="24.90625" customWidth="1"/>
     <col min="15" max="15" width="29.26953125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="30.90625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="39.08984375" customWidth="1"/>
+    <col min="17" max="17" width="29.26953125" customWidth="1"/>
     <col min="18" max="19" width="32.90625" customWidth="1"/>
-    <col min="20" max="20" width="23.90625" customWidth="1"/>
-    <col min="21" max="22" width="28.26953125" customWidth="1"/>
-    <col min="23" max="23" width="23.26953125" customWidth="1"/>
+    <col min="20" max="20" width="22.08984375" customWidth="1"/>
+    <col min="21" max="21" width="25.81640625" customWidth="1"/>
+    <col min="22" max="22" width="25.7265625" customWidth="1"/>
+    <col min="23" max="23" width="21.36328125" customWidth="1"/>
     <col min="24" max="24" width="20.453125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="24.6328125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="28.1796875" customWidth="1"/>
+    <col min="26" max="26" width="26.54296875" customWidth="1"/>
     <col min="27" max="27" width="59" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -717,7 +718,7 @@
         <v>29</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>63</v>
@@ -726,13 +727,13 @@
         <v>28</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>58</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>62</v>
@@ -741,37 +742,37 @@
         <v>27</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N1" s="4" t="s">
         <v>26</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>64</v>
+        <v>91</v>
       </c>
       <c r="Q1" s="4" t="s">
         <v>59</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T1" s="4" t="s">
         <v>60</v>
       </c>
       <c r="U1" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="V1" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="W1" s="4" t="s">
         <v>56</v>
@@ -912,7 +913,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D3">
         <v>12.5</v>
@@ -937,7 +938,7 @@
         <v>3</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L3">
         <v>115</v>
@@ -1191,7 +1192,7 @@
         <v>200</v>
       </c>
       <c r="Q5" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="R5">
         <v>77.5</v>
@@ -1201,7 +1202,7 @@
         <v>232.5</v>
       </c>
       <c r="T5" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="U5">
         <v>450</v>
@@ -1260,7 +1261,7 @@
         <v>21</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>7</v>
@@ -1405,7 +1406,7 @@
         <v>4</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L7">
         <v>130</v>
@@ -1494,7 +1495,7 @@
         <v>21</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>8</v>
@@ -1522,7 +1523,7 @@
         <v>3</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L8">
         <v>125</v>
@@ -1614,7 +1615,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D9">
         <v>12.5</v>
@@ -1639,7 +1640,7 @@
         <v>1</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L9">
         <v>80</v>
@@ -1873,7 +1874,7 @@
         <v>3</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L11">
         <v>145</v>
@@ -2147,7 +2148,7 @@
         <v>45</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="306.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2155,7 +2156,7 @@
         <v>35</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -2172,7 +2173,7 @@
         <v>58</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="85" customHeight="1" x14ac:dyDescent="0.3">
@@ -2183,20 +2184,20 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="163" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="188" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="213" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="225.5" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="263" x14ac:dyDescent="0.3">
@@ -2204,7 +2205,7 @@
         <v>24</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="250.5" x14ac:dyDescent="0.3">
@@ -2212,7 +2213,7 @@
         <v>25</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="213" x14ac:dyDescent="0.3">
@@ -2220,7 +2221,7 @@
         <v>56</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="144" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
New Plot zu Raumbedarf und Umweltwirkung
</commit_message>
<xml_diff>
--- a/00_data_raw/Rohdaten_Matrix_Belaege.xlsx
+++ b/00_data_raw/Rohdaten_Matrix_Belaege.xlsx
@@ -673,8 +673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69245AB7-8A4B-4C00-997D-6D46C1094D77}">
   <dimension ref="A1:BF27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="V10" sqref="V10"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fix Plots bäume_leistung-clean and baeume_raumbedarf-clean
</commit_message>
<xml_diff>
--- a/00_data_raw/Rohdaten_Matrix_Belaege.xlsx
+++ b/00_data_raw/Rohdaten_Matrix_Belaege.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://zhaw-my.sharepoint.com/personal/pfeifsar_students_zhaw_ch/Documents/6. Semester MSc UnR/Thesis/R_Project/00_data_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1339" documentId="8_{E9D6D6FE-F378-4AF9-A02F-B79ECDA22C50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B64FD6C6-45CC-43BA-B4BA-2B06C5C252B3}"/>
+  <xr:revisionPtr revIDLastSave="1341" documentId="8_{E9D6D6FE-F378-4AF9-A02F-B79ECDA22C50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A055517-984A-4A41-9BE5-D91D09D5DD6A}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="93">
   <si>
     <t>Modulare Erneuerbarkeit</t>
   </si>
@@ -228,9 +228,6 @@
   </si>
   <si>
     <t>Anzahl Erneuerungen [100a]</t>
-  </si>
-  <si>
-    <t>Kosten [CHF/m²100a]</t>
   </si>
   <si>
     <t>CO₂-Emissionen [kg CO₂-eq/m²100a]</t>
@@ -335,6 +332,12 @@
   </si>
   <si>
     <t>Unterhaltskosten [CHF/CHF/m²100a]</t>
+  </si>
+  <si>
+    <t>Initialkosten [CHF/m²]</t>
+  </si>
+  <si>
+    <t>Initialkosten [CHF/m²100a]</t>
   </si>
 </sst>
 </file>
@@ -673,8 +676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69245AB7-8A4B-4C00-997D-6D46C1094D77}">
   <dimension ref="A1:BF27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -718,7 +721,7 @@
         <v>29</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>63</v>
@@ -727,52 +730,52 @@
         <v>28</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>58</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>62</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>27</v>
+        <v>91</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>64</v>
+        <v>92</v>
       </c>
       <c r="N1" s="4" t="s">
         <v>26</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q1" s="4" t="s">
         <v>59</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="T1" s="4" t="s">
         <v>60</v>
       </c>
       <c r="U1" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="V1" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="W1" s="4" t="s">
         <v>56</v>
@@ -913,7 +916,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D3">
         <v>12.5</v>
@@ -938,7 +941,7 @@
         <v>3</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L3">
         <v>115</v>
@@ -1192,7 +1195,7 @@
         <v>200</v>
       </c>
       <c r="Q5" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="R5">
         <v>77.5</v>
@@ -1202,7 +1205,7 @@
         <v>232.5</v>
       </c>
       <c r="T5" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="U5">
         <v>450</v>
@@ -1261,7 +1264,7 @@
         <v>21</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>7</v>
@@ -1406,7 +1409,7 @@
         <v>4</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L7">
         <v>130</v>
@@ -1495,7 +1498,7 @@
         <v>21</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>8</v>
@@ -1523,7 +1526,7 @@
         <v>3</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L8">
         <v>125</v>
@@ -1615,7 +1618,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D9">
         <v>12.5</v>
@@ -1640,7 +1643,7 @@
         <v>1</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L9">
         <v>80</v>
@@ -1874,7 +1877,7 @@
         <v>3</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L11">
         <v>145</v>
@@ -2148,7 +2151,7 @@
         <v>45</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="306.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2156,7 +2159,7 @@
         <v>35</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -2173,7 +2176,7 @@
         <v>58</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="85" customHeight="1" x14ac:dyDescent="0.3">
@@ -2184,20 +2187,20 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="188" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="163" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="225.5" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="213" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="263" x14ac:dyDescent="0.3">
@@ -2205,7 +2208,7 @@
         <v>24</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="250.5" x14ac:dyDescent="0.3">
@@ -2213,7 +2216,7 @@
         <v>25</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="213" x14ac:dyDescent="0.3">
@@ -2221,7 +2224,7 @@
         <v>56</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="144" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>